<commit_message>
kartu stok dan AP
</commit_message>
<xml_diff>
--- a/doc/Proposal.xlsx
+++ b/doc/Proposal.xlsx
@@ -320,8 +320,8 @@
     <numFmt numFmtId="176" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -356,7 +356,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -370,77 +385,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -470,6 +423,37 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
@@ -477,8 +461,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -507,187 +507,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -716,6 +716,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -727,6 +736,30 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -772,39 +805,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -816,7 +816,7 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -832,130 +832,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1331,11 +1331,11 @@
   <dimension ref="A1:Q64"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C22" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C46" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E33" sqref="E33"/>
+      <selection pane="bottomRight" activeCell="E61" sqref="E61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1982,7 +1982,7 @@
         <v>52</v>
       </c>
       <c r="E23" s="6">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
@@ -2007,7 +2007,7 @@
         <v>54</v>
       </c>
       <c r="E24" s="6">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
@@ -2142,7 +2142,9 @@
       <c r="D30" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="E30" s="6"/>
+      <c r="E30" s="6">
+        <v>100</v>
+      </c>
       <c r="F30" s="6"/>
       <c r="G30" s="6"/>
       <c r="H30" s="6"/>
@@ -2780,7 +2782,9 @@
       <c r="D58" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="E58" s="6"/>
+      <c r="E58" s="6">
+        <v>25</v>
+      </c>
       <c r="F58" s="6"/>
       <c r="G58" s="6"/>
       <c r="H58" s="6"/>

</xml_diff>

<commit_message>
lap ar,ap, retur supplier, karuar, kartu ap
</commit_message>
<xml_diff>
--- a/doc/Proposal.xlsx
+++ b/doc/Proposal.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20385" windowHeight="8370"/>
+    <workbookView windowWidth="19890" windowHeight="8370"/>
   </bookViews>
   <sheets>
     <sheet name="Daftar Fitur" sheetId="1" r:id="rId1"/>
@@ -319,9 +319,9 @@
   <numFmts count="5">
     <numFmt numFmtId="176" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -356,22 +356,21 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -386,7 +385,61 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -401,6 +454,22 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -422,75 +491,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -507,54 +507,144 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -567,19 +657,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -591,7 +669,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -603,91 +687,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -716,11 +716,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -742,39 +748,20 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -797,26 +784,39 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -832,130 +832,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1331,11 +1331,11 @@
   <dimension ref="A1:Q64"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C46" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C14" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E61" sqref="E61"/>
+      <selection pane="bottomRight" activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -2783,7 +2783,7 @@
         <v>88</v>
       </c>
       <c r="E58" s="6">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="F58" s="6"/>
       <c r="G58" s="6"/>
@@ -2805,7 +2805,9 @@
       <c r="D59" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="E59" s="6"/>
+      <c r="E59" s="6">
+        <v>100</v>
+      </c>
       <c r="F59" s="6"/>
       <c r="G59" s="6"/>
       <c r="H59" s="6"/>

</xml_diff>